<commit_message>
Adding KiCad files for a PCB AntiMonitor board
</commit_message>
<xml_diff>
--- a/Boards.xlsx
+++ b/Boards.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A554403-07B0-49D2-B8EF-2189CD4C5318}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21975" windowHeight="11205" activeTab="5"/>
+    <workbookView xWindow="3075" yWindow="360" windowWidth="21615" windowHeight="14265" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Board 64K" sheetId="11" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5153" uniqueCount="1097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5150" uniqueCount="1099">
   <si>
     <t>A11</t>
   </si>
@@ -3321,12 +3322,18 @@
   </si>
   <si>
     <t>Secondary Master</t>
+  </si>
+  <si>
+    <t>/SYSBUS</t>
+  </si>
+  <si>
+    <t>System Bus Enabled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
@@ -4909,33 +4916,195 @@
   <dxfs count="151">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -6258,6 +6427,42 @@
       </fill>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -6319,231 +6524,33 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6573,60 +6580,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:H8" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A2:H8" totalsRowShown="0">
   <tableColumns count="8">
-    <tableColumn id="1" name="B0"/>
-    <tableColumn id="2" name="B1"/>
-    <tableColumn id="3" name="B2"/>
-    <tableColumn id="4" name="B3"/>
-    <tableColumn id="5" name="Q"/>
-    <tableColumn id="8" name="Mem1" dataDxfId="150"/>
-    <tableColumn id="9" name="Mem2"/>
-    <tableColumn id="10" name="Rom"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="B0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="B1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="B2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="B3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Q"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Mem1" dataDxfId="141"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Mem2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Rom"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A19:F22" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table145" displayName="Table145" ref="A19:F22" totalsRowShown="0">
   <tableColumns count="6">
-    <tableColumn id="1" name="/B0"/>
-    <tableColumn id="2" name="Q"/>
-    <tableColumn id="3" name="/Rom" dataDxfId="149"/>
-    <tableColumn id="4" name="/MemB"/>
-    <tableColumn id="5" name="NC1"/>
-    <tableColumn id="8" name="NC2" dataDxfId="148"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="/B0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Q"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="/Rom" dataDxfId="140"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="/MemB"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="NC1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="NC2" dataDxfId="139"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J9" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A2:J9" totalsRowShown="0">
   <tableColumns count="10">
-    <tableColumn id="1" name="B0"/>
-    <tableColumn id="2" name="B1"/>
-    <tableColumn id="3" name="B2"/>
-    <tableColumn id="4" name="B3"/>
-    <tableColumn id="5" name="MA19"/>
-    <tableColumn id="6" name="Q"/>
-    <tableColumn id="7" name="/Q"/>
-    <tableColumn id="8" name="Mem1" dataDxfId="147"/>
-    <tableColumn id="9" name="Mem2"/>
-    <tableColumn id="10" name="Rom"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="B0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="B1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="B2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="B3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="MA19"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Q"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="/Q"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Mem1" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Mem2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Rom"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A26:D30" totalsRowShown="0" dataDxfId="146" tableBorderDxfId="145">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table2" displayName="Table2" ref="A26:D30" totalsRowShown="0" dataDxfId="5" tableBorderDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" name="Mem1-0" dataDxfId="144"/>
-    <tableColumn id="2" name="Mem1-1" dataDxfId="143"/>
-    <tableColumn id="3" name="Mem1-23" dataDxfId="142"/>
-    <tableColumn id="4" name="Mem1CE" dataDxfId="141"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Mem1-0" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Mem1-1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Mem1-23" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Mem1CE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6894,7 +6901,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7720,35 +7727,35 @@
     <mergeCell ref="K37:L50"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:H8">
-    <cfRule type="cellIs" dxfId="140" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="118" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="119" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="120" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:E22">
-    <cfRule type="cellIs" dxfId="137" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="5" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="6" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F22">
-    <cfRule type="cellIs" dxfId="134" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="2" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="3" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7762,7 +7769,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
@@ -9372,7 +9379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J118"/>
   <sheetViews>
     <sheetView topLeftCell="A91" workbookViewId="0">
@@ -11776,7 +11783,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G134"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
@@ -13455,7 +13462,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13916,68 +13923,68 @@
     <mergeCell ref="F9:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="A44:C45">
-    <cfRule type="cellIs" dxfId="131" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="16" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="17" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="18" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:E10 E11">
-    <cfRule type="cellIs" dxfId="128" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="14" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="15" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5 F7 F9">
-    <cfRule type="cellIs" dxfId="125" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="10" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="11" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="12" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="122" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="7" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="8" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="9" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:D11">
-    <cfRule type="cellIs" dxfId="119" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="5" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="6" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="116" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="2" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="3" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13987,7 +13994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:N93"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -15349,420 +15356,420 @@
     <mergeCell ref="F65:F67"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:J5 A7:J8">
-    <cfRule type="cellIs" dxfId="113" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="136" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="137" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="138" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:J6">
-    <cfRule type="cellIs" dxfId="110" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="133" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="134" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="135" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A14">
-    <cfRule type="cellIs" dxfId="107" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="130" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="131" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="132" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="cellIs" dxfId="104" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="91" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="92" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="93" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:E23">
-    <cfRule type="cellIs" dxfId="101" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="79" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="80" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="81" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C14">
-    <cfRule type="cellIs" dxfId="98" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="124" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="125" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="126" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D14">
-    <cfRule type="cellIs" dxfId="95" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="118" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="119" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="120" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B19">
-    <cfRule type="cellIs" dxfId="92" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="103" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="104" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="105" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E14">
-    <cfRule type="cellIs" dxfId="89" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="112" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="113" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="114" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:A19">
-    <cfRule type="cellIs" dxfId="86" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="106" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="107" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="108" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="cellIs" dxfId="83" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="85" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="86" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="87" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C19">
-    <cfRule type="cellIs" dxfId="80" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="100" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="101" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="102" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="cellIs" dxfId="77" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="94" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="95" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="96" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="cellIs" dxfId="74" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="88" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="89" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="90" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="71" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="67" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="68" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="69" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:E22">
-    <cfRule type="cellIs" dxfId="68" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="82" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="83" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="84" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="cellIs" dxfId="65" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="70" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="71" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="72" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:E24">
-    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="64" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="65" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="66" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:J9">
-    <cfRule type="cellIs" dxfId="59" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="58" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="59" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="60" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="56" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="10" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="11" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="12" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="55" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="56" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="57" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="52" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="53" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="54" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="49" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="50" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="51" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="47" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="48" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="43" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="44" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="45" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="40" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="41" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="42" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="37" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="38" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="39" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="34" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="35" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="36" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="31" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="32" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="28" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="29" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="30" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="26" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="22" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="23" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="19" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="20" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="17" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15776,7 +15783,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16057,7 +16064,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16070,11 +16077,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="D1:V424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
-      <selection activeCell="D424" sqref="D424"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="P150" sqref="P150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19581,9 +19588,7 @@
       <c r="I144" s="201" t="s">
         <v>63</v>
       </c>
-      <c r="J144" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="J144" s="3"/>
     </row>
     <row r="145" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D145" s="1" t="s">
@@ -19693,10 +19698,12 @@
       <c r="H149" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I149" s="201" t="s">
-        <v>63</v>
-      </c>
-      <c r="J149" s="177"/>
+      <c r="I149" s="91" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J149" s="4" t="s">
+        <v>1098</v>
+      </c>
     </row>
     <row r="150" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D150" s="1" t="s">
@@ -19736,7 +19743,6 @@
       <c r="I151" s="201" t="s">
         <v>63</v>
       </c>
-      <c r="J151" s="4"/>
     </row>
     <row r="152" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E152" s="15" t="s">
@@ -19792,9 +19798,7 @@
       <c r="I154" s="201" t="s">
         <v>63</v>
       </c>
-      <c r="J154" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="J154" s="4"/>
     </row>
     <row r="155" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D155" s="1" t="s">
@@ -19815,9 +19819,7 @@
       <c r="I155" s="201" t="s">
         <v>63</v>
       </c>
-      <c r="J155" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="J155" s="4"/>
     </row>
     <row r="156" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D156" s="1" t="s">
@@ -19838,9 +19840,7 @@
       <c r="I156" s="201" t="s">
         <v>63</v>
       </c>
-      <c r="J156" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="J156" s="4"/>
     </row>
     <row r="157" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D157" s="1" t="s">
@@ -19861,16 +19861,14 @@
       <c r="I157" s="201" t="s">
         <v>63</v>
       </c>
-      <c r="J157" s="4" t="s">
-        <v>1068</v>
-      </c>
+      <c r="J157" s="4"/>
     </row>
     <row r="158" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D158" s="176" t="s">
         <v>621</v>
       </c>
       <c r="E158" s="16" t="s">
-        <v>620</v>
+        <v>735</v>
       </c>
       <c r="F158" s="6" t="s">
         <v>49</v>
@@ -19893,7 +19891,7 @@
         <v>622</v>
       </c>
       <c r="E159" s="16" t="s">
-        <v>582</v>
+        <v>736</v>
       </c>
       <c r="F159" s="6" t="s">
         <v>49</v>
@@ -19916,7 +19914,7 @@
         <v>623</v>
       </c>
       <c r="E160" s="16" t="s">
-        <v>583</v>
+        <v>737</v>
       </c>
       <c r="F160" s="6" t="s">
         <v>49</v>
@@ -19939,7 +19937,7 @@
         <v>624</v>
       </c>
       <c r="E161" s="16" t="s">
-        <v>584</v>
+        <v>744</v>
       </c>
       <c r="F161" s="6" t="s">
         <v>49</v>
@@ -19962,7 +19960,7 @@
         <v>625</v>
       </c>
       <c r="E162" s="16" t="s">
-        <v>585</v>
+        <v>743</v>
       </c>
       <c r="F162" s="6" t="s">
         <v>49</v>
@@ -19985,7 +19983,7 @@
         <v>626</v>
       </c>
       <c r="E163" s="16" t="s">
-        <v>586</v>
+        <v>742</v>
       </c>
       <c r="F163" s="6" t="s">
         <v>49</v>
@@ -20008,7 +20006,7 @@
         <v>627</v>
       </c>
       <c r="E164" s="16" t="s">
-        <v>588</v>
+        <v>741</v>
       </c>
       <c r="F164" s="6" t="s">
         <v>49</v>
@@ -20031,7 +20029,7 @@
         <v>628</v>
       </c>
       <c r="E165" s="16" t="s">
-        <v>587</v>
+        <v>740</v>
       </c>
       <c r="F165" s="6" t="s">
         <v>49</v>
@@ -20429,8 +20427,11 @@
       <c r="H185" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I185" s="201" t="s">
-        <v>63</v>
+      <c r="I185" s="91" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J185" s="4" t="s">
+        <v>1098</v>
       </c>
     </row>
     <row r="186" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -25607,7 +25608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J121"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
@@ -28062,7 +28063,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -29277,7 +29278,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G165"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">

</xml_diff>